<commit_message>
Orange illustration and data science analytics done
</commit_message>
<xml_diff>
--- a/dataset/movie-tweets/squid game-label.xlsx
+++ b/dataset/movie-tweets/squid game-label.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaqinayasmin/Desktop/cancelled/dataset/movie-tweets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\vin\Projects\cancelled\dataset\movie-tweets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6394F0A4-4B2B-46D5-A1A4-781504471981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="21160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$508</definedName>
+  </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -1850,7 +1854,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1911,77 +1915,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2271,19 +2210,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B482" zoomScale="155" zoomScaleNormal="155" zoomScalePageLayoutView="155" workbookViewId="0">
-      <selection activeCell="B355" sqref="B355"/>
+    <sheetView tabSelected="1" topLeftCell="A478" zoomScaleNormal="100" zoomScalePageLayoutView="155" workbookViewId="0">
+      <selection activeCell="B508" sqref="B508"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="134.83203125" customWidth="1"/>
+    <col min="2" max="2" width="134.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2291,7 +2230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2302,7 +2241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2313,7 +2252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2324,7 +2263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2335,7 +2274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2346,7 +2285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2357,7 +2296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2365,10 +2304,10 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2376,10 +2315,10 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2390,7 +2329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2401,7 +2340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2412,7 +2351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2423,7 +2362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2434,7 +2373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2445,7 +2384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2456,7 +2395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2467,7 +2406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2478,7 +2417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2489,7 +2428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2500,7 +2439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2511,7 +2450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2522,7 +2461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2533,7 +2472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2544,7 +2483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2555,7 +2494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2566,7 +2505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2574,10 +2513,10 @@
         <v>27</v>
       </c>
       <c r="C27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2588,7 +2527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2599,7 +2538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2610,7 +2549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2621,7 +2560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2632,7 +2571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2643,7 +2582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2654,7 +2593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2662,10 +2601,10 @@
         <v>35</v>
       </c>
       <c r="C35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2676,7 +2615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2687,7 +2626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2698,7 +2637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2709,7 +2648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2720,7 +2659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2731,7 +2670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2742,7 +2681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2753,7 +2692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2764,7 +2703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2775,7 +2714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2786,7 +2725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2797,7 +2736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2805,10 +2744,10 @@
         <v>48</v>
       </c>
       <c r="C48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2819,7 +2758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2830,7 +2769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2841,7 +2780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2852,7 +2791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2863,7 +2802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2874,7 +2813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2885,7 +2824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2896,7 +2835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2907,7 +2846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2918,7 +2857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2926,10 +2865,10 @@
         <v>59</v>
       </c>
       <c r="C59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2940,7 +2879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2951,7 +2890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2962,7 +2901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2973,7 +2912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2984,7 +2923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2992,10 +2931,10 @@
         <v>65</v>
       </c>
       <c r="C65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -3006,7 +2945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -3017,7 +2956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -3028,7 +2967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -3039,7 +2978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -3050,7 +2989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -3061,7 +3000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -3069,10 +3008,10 @@
         <v>72</v>
       </c>
       <c r="C72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -3083,7 +3022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -3094,7 +3033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -3105,7 +3044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -3116,7 +3055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -3127,7 +3066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -3138,7 +3077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -3149,7 +3088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -3157,10 +3096,10 @@
         <v>80</v>
       </c>
       <c r="C80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -3171,7 +3110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -3182,7 +3121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -3193,7 +3132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -3204,7 +3143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -3215,7 +3154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -3226,7 +3165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -3237,7 +3176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -3248,7 +3187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -3259,7 +3198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -3270,7 +3209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -3281,7 +3220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -3292,7 +3231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -3303,7 +3242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -3314,7 +3253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -3325,7 +3264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -3336,7 +3275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -3347,7 +3286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -3358,7 +3297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -3369,7 +3308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -3380,7 +3319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -3391,7 +3330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -3402,7 +3341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -3413,7 +3352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -3424,7 +3363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -3435,7 +3374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -3446,7 +3385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -3457,7 +3396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -3468,7 +3407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -3479,7 +3418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -3490,7 +3429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -3501,7 +3440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -3512,7 +3451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -3523,7 +3462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -3534,7 +3473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -3545,7 +3484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -3556,7 +3495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -3567,7 +3506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -3578,7 +3517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -3589,7 +3528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -3600,7 +3539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -3611,7 +3550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -3622,7 +3561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -3633,7 +3572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -3644,7 +3583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -3655,7 +3594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -3666,7 +3605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -3677,7 +3616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -3688,7 +3627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -3699,7 +3638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -3710,7 +3649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -3721,7 +3660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -3732,7 +3671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -3743,7 +3682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -3754,7 +3693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -3765,7 +3704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -3776,7 +3715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -3787,7 +3726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -3798,7 +3737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -3809,7 +3748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -3820,7 +3759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -3831,7 +3770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -3842,7 +3781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -3853,7 +3792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -3864,7 +3803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -3875,7 +3814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -3886,7 +3825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -3897,7 +3836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -3908,7 +3847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -3919,7 +3858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -3930,7 +3869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -3941,7 +3880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -3952,7 +3891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -3963,7 +3902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -3974,7 +3913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -3985,7 +3924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -3996,7 +3935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -4007,7 +3946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -4018,7 +3957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -4029,7 +3968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -4040,7 +3979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -4051,7 +3990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -4062,7 +4001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -4073,7 +4012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -4084,7 +4023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -4095,7 +4034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -4106,7 +4045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -4117,7 +4056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -4128,7 +4067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -4139,7 +4078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -4150,7 +4089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -4161,7 +4100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -4172,7 +4111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -4183,7 +4122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -4194,7 +4133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -4205,7 +4144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -4216,7 +4155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -4227,7 +4166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -4238,7 +4177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -4249,7 +4188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -4260,7 +4199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -4271,7 +4210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -4282,7 +4221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -4293,7 +4232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -4304,7 +4243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -4315,7 +4254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -4326,7 +4265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -4337,7 +4276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -4348,7 +4287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -4359,7 +4298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -4370,7 +4309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -4378,10 +4317,10 @@
         <v>191</v>
       </c>
       <c r="C191">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -4392,7 +4331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -4403,7 +4342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -4414,7 +4353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -4425,7 +4364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -4436,7 +4375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -4447,7 +4386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -4458,7 +4397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -4469,7 +4408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -4480,7 +4419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -4491,7 +4430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -4502,7 +4441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -4513,7 +4452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -4524,7 +4463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -4535,7 +4474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -4546,7 +4485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -4557,7 +4496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -4568,7 +4507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -4579,7 +4518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -4590,7 +4529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -4601,7 +4540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -4612,7 +4551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -4623,7 +4562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -4634,7 +4573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -4645,7 +4584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -4656,7 +4595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -4667,7 +4606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>216</v>
       </c>
@@ -4678,7 +4617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -4689,7 +4628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -4700,7 +4639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>219</v>
       </c>
@@ -4711,7 +4650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -4722,7 +4661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -4733,7 +4672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>222</v>
       </c>
@@ -4744,7 +4683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -4755,7 +4694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -4766,7 +4705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -4777,7 +4716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -4788,7 +4727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -4799,7 +4738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -4810,7 +4749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -4821,7 +4760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -4832,7 +4771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>231</v>
       </c>
@@ -4843,7 +4782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -4854,7 +4793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>233</v>
       </c>
@@ -4865,7 +4804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>234</v>
       </c>
@@ -4876,7 +4815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -4887,7 +4826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -4898,7 +4837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -4909,7 +4848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -4920,7 +4859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -4931,7 +4870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -4942,7 +4881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -4953,7 +4892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -4964,7 +4903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -4975,7 +4914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -4986,7 +4925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -4997,7 +4936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>246</v>
       </c>
@@ -5008,7 +4947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>247</v>
       </c>
@@ -5019,7 +4958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>248</v>
       </c>
@@ -5030,7 +4969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>249</v>
       </c>
@@ -5041,7 +4980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -5052,7 +4991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>251</v>
       </c>
@@ -5063,7 +5002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>252</v>
       </c>
@@ -5074,7 +5013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>253</v>
       </c>
@@ -5085,7 +5024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>254</v>
       </c>
@@ -5096,7 +5035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>255</v>
       </c>
@@ -5107,7 +5046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>256</v>
       </c>
@@ -5118,7 +5057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>257</v>
       </c>
@@ -5129,7 +5068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>258</v>
       </c>
@@ -5140,7 +5079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>259</v>
       </c>
@@ -5151,7 +5090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>260</v>
       </c>
@@ -5162,7 +5101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>261</v>
       </c>
@@ -5173,7 +5112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>262</v>
       </c>
@@ -5184,7 +5123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>263</v>
       </c>
@@ -5195,7 +5134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>264</v>
       </c>
@@ -5206,7 +5145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>265</v>
       </c>
@@ -5217,7 +5156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>266</v>
       </c>
@@ -5225,10 +5164,10 @@
         <v>268</v>
       </c>
       <c r="C268">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>267</v>
       </c>
@@ -5239,7 +5178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>268</v>
       </c>
@@ -5250,7 +5189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>269</v>
       </c>
@@ -5261,7 +5200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>270</v>
       </c>
@@ -5272,7 +5211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>271</v>
       </c>
@@ -5283,7 +5222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>272</v>
       </c>
@@ -5294,7 +5233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>273</v>
       </c>
@@ -5305,7 +5244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>274</v>
       </c>
@@ -5316,7 +5255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>275</v>
       </c>
@@ -5327,7 +5266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>276</v>
       </c>
@@ -5338,7 +5277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>277</v>
       </c>
@@ -5349,7 +5288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>278</v>
       </c>
@@ -5360,7 +5299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>279</v>
       </c>
@@ -5371,7 +5310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>280</v>
       </c>
@@ -5382,7 +5321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>281</v>
       </c>
@@ -5390,10 +5329,10 @@
         <v>283</v>
       </c>
       <c r="C283">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>282</v>
       </c>
@@ -5404,7 +5343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>283</v>
       </c>
@@ -5415,7 +5354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>284</v>
       </c>
@@ -5426,7 +5365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>285</v>
       </c>
@@ -5437,7 +5376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>286</v>
       </c>
@@ -5448,7 +5387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>287</v>
       </c>
@@ -5459,7 +5398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>288</v>
       </c>
@@ -5470,7 +5409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>289</v>
       </c>
@@ -5481,7 +5420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>290</v>
       </c>
@@ -5489,10 +5428,10 @@
         <v>292</v>
       </c>
       <c r="C292">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>291</v>
       </c>
@@ -5503,7 +5442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>292</v>
       </c>
@@ -5514,7 +5453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>293</v>
       </c>
@@ -5525,7 +5464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>294</v>
       </c>
@@ -5536,7 +5475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>295</v>
       </c>
@@ -5547,7 +5486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>296</v>
       </c>
@@ -5558,7 +5497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>297</v>
       </c>
@@ -5569,7 +5508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>298</v>
       </c>
@@ -5580,7 +5519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>299</v>
       </c>
@@ -5591,7 +5530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>300</v>
       </c>
@@ -5602,7 +5541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>301</v>
       </c>
@@ -5613,7 +5552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>302</v>
       </c>
@@ -5624,7 +5563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>303</v>
       </c>
@@ -5635,7 +5574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>304</v>
       </c>
@@ -5646,7 +5585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>305</v>
       </c>
@@ -5657,7 +5596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>306</v>
       </c>
@@ -5668,7 +5607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>307</v>
       </c>
@@ -5679,7 +5618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>308</v>
       </c>
@@ -5690,7 +5629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>309</v>
       </c>
@@ -5701,7 +5640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>310</v>
       </c>
@@ -5712,7 +5651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>311</v>
       </c>
@@ -5720,10 +5659,10 @@
         <v>313</v>
       </c>
       <c r="C313">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>312</v>
       </c>
@@ -5734,7 +5673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>313</v>
       </c>
@@ -5745,7 +5684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>314</v>
       </c>
@@ -5756,7 +5695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <v>315</v>
       </c>
@@ -5764,10 +5703,10 @@
         <v>317</v>
       </c>
       <c r="C317">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <v>316</v>
       </c>
@@ -5778,7 +5717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
         <v>317</v>
       </c>
@@ -5789,7 +5728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
         <v>318</v>
       </c>
@@ -5800,7 +5739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321" s="1">
         <v>319</v>
       </c>
@@ -5811,7 +5750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322" s="1">
         <v>320</v>
       </c>
@@ -5822,7 +5761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
         <v>321</v>
       </c>
@@ -5833,7 +5772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" s="1">
         <v>322</v>
       </c>
@@ -5844,7 +5783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
         <v>323</v>
       </c>
@@ -5855,7 +5794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
         <v>324</v>
       </c>
@@ -5866,7 +5805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" s="1">
         <v>325</v>
       </c>
@@ -5877,7 +5816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" s="1">
         <v>326</v>
       </c>
@@ -5888,7 +5827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" s="1">
         <v>327</v>
       </c>
@@ -5896,10 +5835,10 @@
         <v>329</v>
       </c>
       <c r="C329">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A330" s="1">
         <v>328</v>
       </c>
@@ -5910,7 +5849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331" s="1">
         <v>329</v>
       </c>
@@ -5921,7 +5860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A332" s="1">
         <v>330</v>
       </c>
@@ -5932,7 +5871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333" s="1">
         <v>331</v>
       </c>
@@ -5943,7 +5882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" s="1">
         <v>332</v>
       </c>
@@ -5954,7 +5893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" s="1">
         <v>333</v>
       </c>
@@ -5965,7 +5904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" s="1">
         <v>334</v>
       </c>
@@ -5976,7 +5915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" s="1">
         <v>335</v>
       </c>
@@ -5987,7 +5926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" s="1">
         <v>336</v>
       </c>
@@ -5998,7 +5937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" s="1">
         <v>337</v>
       </c>
@@ -6009,7 +5948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340" s="1">
         <v>338</v>
       </c>
@@ -6020,7 +5959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" s="1">
         <v>339</v>
       </c>
@@ -6031,7 +5970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342" s="1">
         <v>340</v>
       </c>
@@ -6042,7 +5981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A343" s="1">
         <v>341</v>
       </c>
@@ -6050,10 +5989,10 @@
         <v>343</v>
       </c>
       <c r="C343">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A344" s="1">
         <v>342</v>
       </c>
@@ -6064,7 +6003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A345" s="1">
         <v>343</v>
       </c>
@@ -6075,7 +6014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A346" s="1">
         <v>344</v>
       </c>
@@ -6086,7 +6025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A347" s="1">
         <v>345</v>
       </c>
@@ -6097,7 +6036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A348" s="1">
         <v>346</v>
       </c>
@@ -6108,7 +6047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A349" s="1">
         <v>347</v>
       </c>
@@ -6119,7 +6058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A350" s="1">
         <v>348</v>
       </c>
@@ -6130,7 +6069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A351" s="1">
         <v>349</v>
       </c>
@@ -6141,7 +6080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A352" s="1">
         <v>350</v>
       </c>
@@ -6152,7 +6091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A353" s="1">
         <v>351</v>
       </c>
@@ -6163,7 +6102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A354" s="1">
         <v>352</v>
       </c>
@@ -6174,7 +6113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A355" s="1">
         <v>353</v>
       </c>
@@ -6185,7 +6124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A356" s="1">
         <v>354</v>
       </c>
@@ -6196,7 +6135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A357" s="1">
         <v>355</v>
       </c>
@@ -6207,7 +6146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A358" s="1">
         <v>356</v>
       </c>
@@ -6218,7 +6157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A359" s="1">
         <v>357</v>
       </c>
@@ -6229,7 +6168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A360" s="1">
         <v>358</v>
       </c>
@@ -6240,7 +6179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A361" s="1">
         <v>359</v>
       </c>
@@ -6251,7 +6190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A362" s="1">
         <v>360</v>
       </c>
@@ -6262,7 +6201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A363" s="1">
         <v>361</v>
       </c>
@@ -6273,7 +6212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A364" s="1">
         <v>362</v>
       </c>
@@ -6284,7 +6223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A365" s="1">
         <v>363</v>
       </c>
@@ -6295,7 +6234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A366" s="1">
         <v>364</v>
       </c>
@@ -6306,7 +6245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A367" s="1">
         <v>365</v>
       </c>
@@ -6317,7 +6256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A368" s="1">
         <v>366</v>
       </c>
@@ -6328,7 +6267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" s="1">
         <v>367</v>
       </c>
@@ -6339,7 +6278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A370" s="1">
         <v>368</v>
       </c>
@@ -6350,7 +6289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" s="1">
         <v>369</v>
       </c>
@@ -6358,10 +6297,10 @@
         <v>371</v>
       </c>
       <c r="C371">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A372" s="1">
         <v>370</v>
       </c>
@@ -6372,7 +6311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" s="1">
         <v>371</v>
       </c>
@@ -6383,7 +6322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" s="1">
         <v>372</v>
       </c>
@@ -6394,7 +6333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" s="1">
         <v>373</v>
       </c>
@@ -6405,7 +6344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A376" s="1">
         <v>374</v>
       </c>
@@ -6413,10 +6352,10 @@
         <v>376</v>
       </c>
       <c r="C376">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" s="1">
         <v>375</v>
       </c>
@@ -6424,10 +6363,10 @@
         <v>377</v>
       </c>
       <c r="C377">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="378" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A378" s="1">
         <v>376</v>
       </c>
@@ -6435,10 +6374,10 @@
         <v>378</v>
       </c>
       <c r="C378">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="379" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A379" s="1">
         <v>377</v>
       </c>
@@ -6446,10 +6385,10 @@
         <v>379</v>
       </c>
       <c r="C379">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A380" s="1">
         <v>378</v>
       </c>
@@ -6457,10 +6396,10 @@
         <v>380</v>
       </c>
       <c r="C380">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="381" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A381" s="1">
         <v>379</v>
       </c>
@@ -6468,10 +6407,10 @@
         <v>381</v>
       </c>
       <c r="C381">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="382" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A382" s="1">
         <v>380</v>
       </c>
@@ -6482,7 +6421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A383" s="1">
         <v>381</v>
       </c>
@@ -6493,7 +6432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A384" s="1">
         <v>382</v>
       </c>
@@ -6504,7 +6443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A385" s="1">
         <v>383</v>
       </c>
@@ -6515,7 +6454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="386" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A386" s="1">
         <v>384</v>
       </c>
@@ -6526,7 +6465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A387" s="1">
         <v>385</v>
       </c>
@@ -6537,7 +6476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A388" s="1">
         <v>386</v>
       </c>
@@ -6548,7 +6487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A389" s="1">
         <v>387</v>
       </c>
@@ -6559,7 +6498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A390" s="1">
         <v>388</v>
       </c>
@@ -6570,7 +6509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A391" s="1">
         <v>389</v>
       </c>
@@ -6581,7 +6520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A392" s="1">
         <v>390</v>
       </c>
@@ -6592,7 +6531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="393" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A393" s="1">
         <v>391</v>
       </c>
@@ -6603,7 +6542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="394" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A394" s="1">
         <v>392</v>
       </c>
@@ -6614,7 +6553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="395" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A395" s="1">
         <v>393</v>
       </c>
@@ -6625,7 +6564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="396" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A396" s="1">
         <v>394</v>
       </c>
@@ -6636,7 +6575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A397" s="1">
         <v>395</v>
       </c>
@@ -6647,7 +6586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="398" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A398" s="1">
         <v>396</v>
       </c>
@@ -6658,7 +6597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A399" s="1">
         <v>397</v>
       </c>
@@ -6669,7 +6608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="400" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A400" s="1">
         <v>398</v>
       </c>
@@ -6680,7 +6619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A401" s="1">
         <v>399</v>
       </c>
@@ -6691,7 +6630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A402" s="1">
         <v>400</v>
       </c>
@@ -6702,7 +6641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="403" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A403" s="1">
         <v>401</v>
       </c>
@@ -6713,7 +6652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A404" s="1">
         <v>402</v>
       </c>
@@ -6724,7 +6663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="405" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A405" s="1">
         <v>403</v>
       </c>
@@ -6735,7 +6674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="406" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A406" s="1">
         <v>404</v>
       </c>
@@ -6743,10 +6682,10 @@
         <v>406</v>
       </c>
       <c r="C406">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="407" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="407" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A407" s="1">
         <v>405</v>
       </c>
@@ -6757,7 +6696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="408" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A408" s="1">
         <v>406</v>
       </c>
@@ -6768,7 +6707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="409" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A409" s="1">
         <v>407</v>
       </c>
@@ -6779,7 +6718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="410" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A410" s="1">
         <v>408</v>
       </c>
@@ -6790,7 +6729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="411" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A411" s="1">
         <v>409</v>
       </c>
@@ -6801,7 +6740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="412" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A412" s="1">
         <v>410</v>
       </c>
@@ -6812,7 +6751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A413" s="1">
         <v>411</v>
       </c>
@@ -6823,7 +6762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="414" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A414" s="1">
         <v>412</v>
       </c>
@@ -6834,7 +6773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="415" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A415" s="1">
         <v>413</v>
       </c>
@@ -6845,7 +6784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="416" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A416" s="1">
         <v>414</v>
       </c>
@@ -6856,7 +6795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="417" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A417" s="1">
         <v>415</v>
       </c>
@@ -6867,7 +6806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="418" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A418" s="1">
         <v>416</v>
       </c>
@@ -6878,7 +6817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="419" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A419" s="1">
         <v>417</v>
       </c>
@@ -6889,7 +6828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="420" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A420" s="1">
         <v>418</v>
       </c>
@@ -6900,7 +6839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="421" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A421" s="1">
         <v>419</v>
       </c>
@@ -6911,7 +6850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="422" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A422" s="1">
         <v>420</v>
       </c>
@@ -6922,7 +6861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="423" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A423" s="1">
         <v>421</v>
       </c>
@@ -6933,7 +6872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="424" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A424" s="1">
         <v>422</v>
       </c>
@@ -6944,7 +6883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="425" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A425" s="1">
         <v>423</v>
       </c>
@@ -6955,7 +6894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="426" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A426" s="1">
         <v>424</v>
       </c>
@@ -6966,7 +6905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="427" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A427" s="1">
         <v>425</v>
       </c>
@@ -6977,7 +6916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="428" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A428" s="1">
         <v>426</v>
       </c>
@@ -6988,7 +6927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="429" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A429" s="1">
         <v>427</v>
       </c>
@@ -6999,7 +6938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="430" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A430" s="1">
         <v>428</v>
       </c>
@@ -7010,7 +6949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="431" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A431" s="1">
         <v>429</v>
       </c>
@@ -7021,7 +6960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="432" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A432" s="1">
         <v>430</v>
       </c>
@@ -7032,7 +6971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="433" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A433" s="1">
         <v>431</v>
       </c>
@@ -7043,7 +6982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="434" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A434" s="1">
         <v>432</v>
       </c>
@@ -7054,7 +6993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="435" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A435" s="1">
         <v>433</v>
       </c>
@@ -7065,7 +7004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="436" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A436" s="1">
         <v>434</v>
       </c>
@@ -7076,7 +7015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="437" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A437" s="1">
         <v>435</v>
       </c>
@@ -7087,7 +7026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="438" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A438" s="1">
         <v>436</v>
       </c>
@@ -7098,7 +7037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="439" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A439" s="1">
         <v>437</v>
       </c>
@@ -7109,7 +7048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="440" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A440" s="1">
         <v>438</v>
       </c>
@@ -7120,7 +7059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="441" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A441" s="1">
         <v>439</v>
       </c>
@@ -7131,7 +7070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="442" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A442" s="1">
         <v>440</v>
       </c>
@@ -7142,7 +7081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="443" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A443" s="1">
         <v>441</v>
       </c>
@@ -7153,7 +7092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="444" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A444" s="1">
         <v>442</v>
       </c>
@@ -7164,7 +7103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="445" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A445" s="1">
         <v>443</v>
       </c>
@@ -7175,7 +7114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="446" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A446" s="1">
         <v>444</v>
       </c>
@@ -7186,7 +7125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="447" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A447" s="1">
         <v>445</v>
       </c>
@@ -7197,7 +7136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="448" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A448" s="1">
         <v>446</v>
       </c>
@@ -7208,7 +7147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="449" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A449" s="1">
         <v>447</v>
       </c>
@@ -7219,7 +7158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="450" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A450" s="1">
         <v>448</v>
       </c>
@@ -7230,7 +7169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="451" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A451" s="1">
         <v>449</v>
       </c>
@@ -7241,7 +7180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="452" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A452" s="1">
         <v>450</v>
       </c>
@@ -7252,7 +7191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="453" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A453" s="1">
         <v>451</v>
       </c>
@@ -7263,7 +7202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="454" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A454" s="1">
         <v>452</v>
       </c>
@@ -7274,7 +7213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="455" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A455" s="1">
         <v>453</v>
       </c>
@@ -7285,7 +7224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="456" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A456" s="1">
         <v>454</v>
       </c>
@@ -7296,7 +7235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="457" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A457" s="1">
         <v>455</v>
       </c>
@@ -7307,7 +7246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="458" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A458" s="1">
         <v>456</v>
       </c>
@@ -7318,7 +7257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="459" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A459" s="1">
         <v>457</v>
       </c>
@@ -7329,7 +7268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="460" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A460" s="1">
         <v>458</v>
       </c>
@@ -7340,7 +7279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="461" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A461" s="1">
         <v>459</v>
       </c>
@@ -7351,7 +7290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="462" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A462" s="1">
         <v>460</v>
       </c>
@@ -7362,7 +7301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="463" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A463" s="1">
         <v>461</v>
       </c>
@@ -7373,7 +7312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="464" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A464" s="1">
         <v>462</v>
       </c>
@@ -7384,7 +7323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="465" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A465" s="1">
         <v>463</v>
       </c>
@@ -7395,7 +7334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="466" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A466" s="1">
         <v>464</v>
       </c>
@@ -7406,7 +7345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="467" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A467" s="1">
         <v>465</v>
       </c>
@@ -7417,7 +7356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="468" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A468" s="1">
         <v>466</v>
       </c>
@@ -7428,7 +7367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="469" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A469" s="1">
         <v>467</v>
       </c>
@@ -7439,7 +7378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="470" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A470" s="1">
         <v>468</v>
       </c>
@@ -7450,7 +7389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="471" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A471" s="1">
         <v>469</v>
       </c>
@@ -7461,7 +7400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="472" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A472" s="1">
         <v>470</v>
       </c>
@@ -7472,7 +7411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="473" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A473" s="1">
         <v>471</v>
       </c>
@@ -7483,7 +7422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="474" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A474" s="1">
         <v>472</v>
       </c>
@@ -7494,7 +7433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="475" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A475" s="1">
         <v>473</v>
       </c>
@@ -7505,7 +7444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="476" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A476" s="1">
         <v>474</v>
       </c>
@@ -7516,7 +7455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="477" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A477" s="1">
         <v>475</v>
       </c>
@@ -7527,7 +7466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="478" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A478" s="1">
         <v>476</v>
       </c>
@@ -7538,7 +7477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="479" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A479" s="1">
         <v>477</v>
       </c>
@@ -7549,7 +7488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="480" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A480" s="1">
         <v>478</v>
       </c>
@@ -7560,7 +7499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="481" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A481" s="1">
         <v>479</v>
       </c>
@@ -7571,7 +7510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="482" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A482" s="1">
         <v>480</v>
       </c>
@@ -7582,7 +7521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="483" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A483" s="1">
         <v>481</v>
       </c>
@@ -7593,7 +7532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="484" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A484" s="1">
         <v>482</v>
       </c>
@@ -7604,7 +7543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="485" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A485" s="1">
         <v>483</v>
       </c>
@@ -7615,7 +7554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="486" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A486" s="1">
         <v>484</v>
       </c>
@@ -7626,7 +7565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="487" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A487" s="1">
         <v>485</v>
       </c>
@@ -7637,7 +7576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="488" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A488" s="1">
         <v>486</v>
       </c>
@@ -7648,7 +7587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="489" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A489" s="1">
         <v>487</v>
       </c>
@@ -7659,7 +7598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="490" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A490" s="1">
         <v>488</v>
       </c>
@@ -7670,7 +7609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="491" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A491" s="1">
         <v>489</v>
       </c>
@@ -7681,7 +7620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="492" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A492" s="1">
         <v>490</v>
       </c>
@@ -7692,7 +7631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="493" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="493" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A493" s="1">
         <v>491</v>
       </c>
@@ -7703,7 +7642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="494" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="494" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A494" s="1">
         <v>492</v>
       </c>
@@ -7714,7 +7653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="495" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A495" s="1">
         <v>493</v>
       </c>
@@ -7725,7 +7664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="496" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A496" s="1">
         <v>494</v>
       </c>
@@ -7736,7 +7675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="497" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A497" s="1">
         <v>495</v>
       </c>
@@ -7747,7 +7686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="498" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A498" s="1">
         <v>496</v>
       </c>
@@ -7758,7 +7697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="499" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A499" s="1">
         <v>497</v>
       </c>
@@ -7769,7 +7708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="500" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A500" s="1">
         <v>498</v>
       </c>
@@ -7780,7 +7719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="501" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="501" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A501" s="1">
         <v>499</v>
       </c>
@@ -7791,7 +7730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="502" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="502" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A502" s="1">
         <v>500</v>
       </c>
@@ -7802,7 +7741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="503" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="503" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A503" s="1">
         <v>501</v>
       </c>
@@ -7813,7 +7752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="504" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="504" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A504" s="1">
         <v>502</v>
       </c>
@@ -7824,7 +7763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="505" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="505" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A505" s="1">
         <v>503</v>
       </c>
@@ -7835,7 +7774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="506" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="506" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A506" s="1">
         <v>504</v>
       </c>
@@ -7846,7 +7785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="507" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="507" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A507" s="1">
         <v>505</v>
       </c>
@@ -7857,7 +7796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="508" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="508" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A508" s="1">
         <v>506</v>
       </c>
@@ -7869,6 +7808,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C508" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>